<commit_message>
added pres, senate seats & house seats to shutdown xls
</commit_message>
<xml_diff>
--- a/Input/government_shutdown_stats.xlsx
+++ b/Input/government_shutdown_stats.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg_\Data-Bootcamp-Project-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\# Gregs Temp\Rice U DABC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3BD04B6-1DAB-4E31-852D-C19A328A4E89}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F60EB91-BEF0-405D-9874-7042060E44D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8865" xr2:uid="{7C7ECD33-EE7F-4020-B0A8-7EC1C6714FF7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="77">
   <si>
     <t>from_date</t>
   </si>
@@ -172,6 +172,96 @@
   </si>
   <si>
     <t>length_in_days</t>
+  </si>
+  <si>
+    <t>president</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>senate_seats</t>
+  </si>
+  <si>
+    <t>house_seats</t>
+  </si>
+  <si>
+    <t>62 - 38</t>
+  </si>
+  <si>
+    <t>291 - 144</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>59 - 41</t>
+  </si>
+  <si>
+    <t>292 - 143</t>
+  </si>
+  <si>
+    <t>58 - 42</t>
+  </si>
+  <si>
+    <t>277 - 158</t>
+  </si>
+  <si>
+    <t>Reagan</t>
+  </si>
+  <si>
+    <t>53 - 47</t>
+  </si>
+  <si>
+    <t>244 - 191</t>
+  </si>
+  <si>
+    <t>55 - 45</t>
+  </si>
+  <si>
+    <t>271 - 164</t>
+  </si>
+  <si>
+    <t>270 - 165</t>
+  </si>
+  <si>
+    <t>253 - 182</t>
+  </si>
+  <si>
+    <t>54 - 46</t>
+  </si>
+  <si>
+    <t>258 - 177</t>
+  </si>
+  <si>
+    <t>G. H. W. Bush</t>
+  </si>
+  <si>
+    <t>258 - 176</t>
+  </si>
+  <si>
+    <t>Clinton</t>
+  </si>
+  <si>
+    <t>233 - 199</t>
+  </si>
+  <si>
+    <t>235 - 198</t>
+  </si>
+  <si>
+    <t>Obama</t>
+  </si>
+  <si>
+    <t>232 - 200</t>
+  </si>
+  <si>
+    <t>Trump</t>
+  </si>
+  <si>
+    <t>51 - 49</t>
+  </si>
+  <si>
+    <t>238 - 193</t>
   </si>
 </sst>
 </file>
@@ -529,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1910A4C6-8E14-4909-A700-38A3DB967E24}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,11 +632,15 @@
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -563,13 +657,22 @@
         <v>41</v>
       </c>
       <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -587,13 +690,22 @@
         <v>44</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -612,13 +724,22 @@
         <v>45</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A21" si="1">A3+1</f>
         <v>3</v>
@@ -637,13 +758,22 @@
         <v>45</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -662,13 +792,22 @@
         <v>45</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -687,13 +826,22 @@
         <v>45</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -712,13 +860,22 @@
         <v>45</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -737,13 +894,22 @@
         <v>44</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -762,13 +928,22 @@
         <v>44</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -787,13 +962,22 @@
         <v>44</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -812,13 +996,22 @@
         <v>44</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -837,13 +1030,22 @@
         <v>44</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -862,13 +1064,22 @@
         <v>44</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -887,13 +1098,22 @@
         <v>44</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -912,13 +1132,22 @@
         <v>44</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -937,13 +1166,22 @@
         <v>44</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -962,13 +1200,22 @@
         <v>45</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -987,13 +1234,22 @@
         <v>45</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1012,13 +1268,22 @@
         <v>45</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1037,13 +1302,22 @@
         <v>44</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1062,10 +1336,19 @@
         <v>44</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>44</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>